<commit_message>
Modificación de documentos y creación de diagramas de flujo para los casos de prueba
</commit_message>
<xml_diff>
--- a/8-Bugtracker.xlsx
+++ b/8-Bugtracker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Choucair\Capacitación\Plan_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Choucair\Capacitación\Plan_2\Ejercicio Práctico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A50EAA-FD4A-4FE6-98E3-C88FFE06FED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A691012-A0DA-4D7D-95D9-97ADE529CA29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Fecha de detección</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>Tipo</t>
-  </si>
-  <si>
-    <t>Descripción</t>
   </si>
   <si>
     <t>Impacto</t>
@@ -111,6 +108,12 @@
 - Login con rol de colaborador
 - Página de búsqueda 
 - Seleccionar la opción de filtro "Universidad Choucair/ Escuela Técnica/ Testing/ Aplicativos"</t>
+  </si>
+  <si>
+    <t>Reporte</t>
+  </si>
+  <si>
+    <t>Severidad</t>
   </si>
 </sst>
 </file>
@@ -568,16 +571,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:R4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" style="3" customWidth="1"/>
     <col min="4" max="4" width="5.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -585,28 +588,28 @@
     <col min="7" max="7" width="16.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="18" style="3" customWidth="1"/>
     <col min="9" max="9" width="32.5703125" style="3" customWidth="1"/>
-    <col min="10" max="11" width="15.28515625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="3"/>
+    <col min="10" max="12" width="15.28515625" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>0</v>
@@ -615,130 +618,136 @@
         <v>1</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="2"/>
+      <c r="M1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="N1" s="2"/>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
     </row>
-    <row r="2" spans="1:17" s="8" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" s="8" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="G2" s="6">
         <v>44971</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J2" s="7">
         <v>2</v>
       </c>
-      <c r="K2" s="7">
+      <c r="K2" s="7"/>
+      <c r="L2" s="7">
         <v>2</v>
       </c>
-      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
     </row>
-    <row r="3" spans="1:17" s="8" customFormat="1" ht="102" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" s="8" customFormat="1" ht="102" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="G3" s="6">
         <v>44971</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J3" s="7">
         <v>1</v>
       </c>
-      <c r="K3" s="7">
+      <c r="K3" s="7"/>
+      <c r="L3" s="7">
         <v>2</v>
       </c>
-      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
     </row>
-    <row r="4" spans="1:17" s="8" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" s="8" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="G4" s="6">
         <v>44971</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J4" s="7">
         <v>1</v>
       </c>
-      <c r="K4" s="7">
+      <c r="K4" s="7"/>
+      <c r="L4" s="7">
         <v>2</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Adición ejemplo Bucktracker en AzureDevOps
</commit_message>
<xml_diff>
--- a/8-Bugtracker.xlsx
+++ b/8-Bugtracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Choucair\Capacitación\Plan_2\Ejercicio Práctico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4730A1A4-5F37-43A8-8B01-5758F2E86756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0EF18B-B652-4F39-98A0-524161F4B0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correcciones de forma en los documentos
</commit_message>
<xml_diff>
--- a/8-Bugtracker.xlsx
+++ b/8-Bugtracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Choucair\Capacitación\Plan_2\Ejercicio Práctico\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0EF18B-B652-4F39-98A0-524161F4B0F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A309518-0373-4170-832A-41609D11A77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -681,8 +681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>

</xml_diff>